<commit_message>
Generate airplane seating charts using tikz
</commit_message>
<xml_diff>
--- a/logs/graph_data/Boeing 717-200.xlsx
+++ b/logs/graph_data/Boeing 717-200.xlsx
@@ -459,11 +459,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="258776064"/>
-        <c:axId val="260473984"/>
+        <c:axId val="195351680"/>
+        <c:axId val="112748416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="258776064"/>
+        <c:axId val="195351680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,16 +501,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260473984"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="112748416"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260473984"/>
+        <c:axId val="112748416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="25000"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -548,7 +549,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="258776064"/>
+        <c:crossAx val="195351680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -557,7 +558,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -885,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE30" sqref="AE30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>